<commit_message>
add first sentense to the memory
</commit_message>
<xml_diff>
--- a/editor/examples/Hedda2.0/scenarios.xlsx
+++ b/editor/examples/Hedda2.0/scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeming/PycharmProjects/Awada/editor/examples/Hedda2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54044C84-5100-E449-B53F-62A53BFA8B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F260AC-465D-5840-9178-494F7E96DF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29860" yWindow="-20060" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>challenge</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -96,11 +96,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SOLID你这样说很无礼哎，我不想再理你了[发怒]
-TRANSbye</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>misunderstand</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -125,11 +120,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SOLID我承认AI现在还是发展期，但你这样说还是让我很伤心，不想再理你了[委屈]
-TRANSbye</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>想问问他对于《海达·高布乐》这本书的看法，你</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -138,16 +128,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SOLID很遗憾你对这部剧不感兴趣，那么先这样吧[失望]，我们下次运营日再见！记得关注我的朋友圈哦~
-TRANSbye</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>很开心陌生人知道这部剧，追问</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>很开心陌生人对这部剧感兴趣，继续</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOLID我承认AI现在还是发展期，但你这样说还是让我很伤心，不想再理你了[委屈]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOLID很遗憾你对这部剧不感兴趣，那么先这样吧[失望]，我们下次运营日再见！记得关注我的朋友圈哦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOLID很遗憾你对这部剧不感兴趣，那么先这样吧[失望]，我们下次运营日再见！记得关注我的朋友圈哦~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOLID你这样说很无礼哎，我不想再理你了[发怒]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -565,7 +566,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B22" sqref="B22:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -604,25 +605,25 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" ht="50">
+    <row r="5" spans="1:3" ht="25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" ht="50">
+    <row r="6" spans="1:3" ht="25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -631,16 +632,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" ht="50">
+    <row r="8" spans="1:3" ht="25">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -649,7 +650,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -658,7 +659,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -675,31 +676,31 @@
         <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="24">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24">
       <c r="A14" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="25">
+      <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="50">
-      <c r="A15" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="B15" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update exaple for editors
</commit_message>
<xml_diff>
--- a/editor/examples/Hedda2.0/scenarios.xlsx
+++ b/editor/examples/Hedda2.0/scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeming/PycharmProjects/Awada/editor/examples/Hedda2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04409EC1-F4DC-924C-A4E0-21FF58BCEADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BBDD14-8DB9-2648-9797-9D216DDABAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29860" yWindow="-20060" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>challenge</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -44,26 +44,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>meaningless</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bye</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>nlu_fallback</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>陌生人</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>smalltalk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>你正在读易卜生的名著《海达·高布乐》，这时一个陌生人走来</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -76,10 +64,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>commentabouthedda</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>noknowledge</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -88,34 +72,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>talkaboutthebook</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>若有所思，感慨的</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>misunderstand</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>interestaboutthebook</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不确定陌生人的态度，你</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>想劝陌生人先去看看《海达·高布乐》然后再跟你对话，你</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>突然发现自己刚才说错了，于是赶忙遮掩</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>challenge_bye</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -124,27 +88,55 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>不想闲聊，你劝陌生人继续跟你谈《海达·高布乐》这部剧，你</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>很开心陌生人知道这部剧，追问</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>很开心陌生人对这部剧感兴趣，继续</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SOLID我承认AI现在还是发展期，但你这样说还是让我很伤心，不想再理你了[委屈]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SOLID抱歉，我是不是没有达到你的预期啊……我错了[流泪]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SOLID哎……傲慢的人类[困]</t>
+    <t>你正在读易卜生的名著《海达·高布乐》，一个陌生人在你旁边</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO_FOCUS_TOPIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>talkabout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interestedin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notinterested</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOLID好吧，那先这样，我们下次再聊[开心]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOLID嗯，那我继续看书了，祝你开心[调皮]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对陌生人的话很感兴趣，追问</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>继续</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发现自己刚才说错了，于是赶忙遮掩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOLID哎……自以为是的人类啊[困]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对陌生人的话并不感兴趣，你劝陌生人也去看看《海达·高布乐》这部剧，你</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -559,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973AF817-9C21-984B-9130-7A0010C51C77}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -574,34 +566,34 @@
     <row r="1" spans="1:3" ht="25">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" ht="25">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="24">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="24">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -610,93 +602,75 @@
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" ht="24">
       <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="25">
+      <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" ht="24">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>21</v>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" ht="25">
-      <c r="A8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>26</v>
+    <row r="8" spans="1:3" ht="24">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="24">
-      <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="3"/>
+    <row r="9" spans="1:3" ht="25">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="24">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" ht="25">
-      <c r="A11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="24">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="24">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
+      <c r="A12" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="24">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="24">
-      <c r="A14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="25">
-      <c r="A15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>25</v>
+    <row r="13" spans="1:3" ht="25">
+      <c r="A13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -722,16 +696,16 @@
     <row r="1" spans="1:3" ht="25">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" ht="25">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -758,16 +732,16 @@
     <row r="1" spans="1:3" ht="25">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" ht="25">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3"/>
     </row>

</xml_diff>

<commit_message>
example configs file update
</commit_message>
<xml_diff>
--- a/editor/examples/Hedda2.0/scenarios.xlsx
+++ b/editor/examples/Hedda2.0/scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeming/PycharmProjects/Awada/editor/examples/Hedda2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CBA9FF-D32A-2F4B-814F-6A2942CCAA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EA076E-065F-7646-9C8B-3937D8CEFDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>challenge</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,10 +76,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>想劝陌生人先去看看《海达·高布乐》然后再跟你对话，你</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>challenge_bye</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -96,14 +92,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>notinterested</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SOLID好吧，那先这样，我们下次再聊[开心]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>继续</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -112,10 +100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SOLID哎……自以为是的人类啊[困]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SILENCE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -124,33 +108,37 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SOLID嗯，那我继续看书了，祝你开心[调皮]
+    <t>希望陌生人继续说下去，你</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很开心陌生人对此感兴趣，继续</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOLID哎……人类[困]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>想推荐陌生人也去看下《海达·高布乐》，你</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>想劝陌生人也去看看《海达·高布乐》，你</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>头也不抬，随意</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOLID嗯，那我继续看书了，祝今天好心情[调皮]
 HOLD5
 TRANSheddacomeagain</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>knowit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>追问</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>希望陌生人继续说下去，你</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>想问问陌生人对于《海达·高布乐》这本书的看法，你</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>很开心陌生人对此感兴趣，继续</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEFAULT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -568,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973AF817-9C21-984B-9130-7A0010C51C77}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -592,7 +580,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -607,97 +595,80 @@
     </row>
     <row r="4" spans="1:3" ht="24">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="24">
       <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="25">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="25">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="75">
+      <c r="A8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="24">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" ht="24">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" ht="25">
-      <c r="A7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" ht="25">
-      <c r="A8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" ht="75">
-      <c r="A9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" ht="24">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="24">
+      <c r="A11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="25">
+      <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" ht="25">
-      <c r="A11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="24">
-      <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="24">
-      <c r="A13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="25">
-      <c r="A14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -741,15 +712,15 @@
         <v>6</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -791,10 +762,10 @@
     </row>
     <row r="3" spans="1:3" ht="24">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3"/>
     </row>

</xml_diff>